<commit_message>
send s3 url to admin
</commit_message>
<xml_diff>
--- a/src/ExcelFile/excel.xlsx
+++ b/src/ExcelFile/excel.xlsx
@@ -442,10 +442,10 @@
         <v>7970206399</v>
       </c>
       <c r="F2" t="str">
-        <v>Yes</v>
+        <v>NO</v>
       </c>
       <c r="G2" t="str">
-        <v>Email sent</v>
+        <v>user already created</v>
       </c>
     </row>
     <row r="3">
@@ -465,10 +465,10 @@
         <v>7970206398</v>
       </c>
       <c r="F3" t="str">
-        <v>Yes</v>
+        <v>NO</v>
       </c>
       <c r="G3" t="str">
-        <v>Email sent</v>
+        <v>user already created</v>
       </c>
     </row>
     <row r="4">
@@ -488,10 +488,10 @@
         <v>7970206395</v>
       </c>
       <c r="F4" t="str">
-        <v>Yes</v>
+        <v>NO</v>
       </c>
       <c r="G4" t="str">
-        <v>Email sent</v>
+        <v>user already created</v>
       </c>
     </row>
   </sheetData>

</xml_diff>